<commit_message>
gestión de adjuntos múltiples corregida
</commit_message>
<xml_diff>
--- a/_encuestas/Calificaciones-2026.xlsx
+++ b/_encuestas/Calificaciones-2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\equih\0 Versiones\Cursos\m3-causalidad\2026\_encuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791FEA0A-06CE-4BB2-AF3E-6041E031E18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8A5C93-EADD-4BDC-A7AD-8930D2DB7072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{57F80845-2267-40DF-BE0E-C1B19A076F2C}"/>
   </bookViews>
@@ -764,7 +764,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1515,7 @@
         <v>8</v>
       </c>
       <c r="H15" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I15" s="1">
         <v>10</v>
@@ -1531,11 +1531,11 @@
       </c>
       <c r="M15" s="2">
         <f>AVERAGE(entregados[[#This Row],[eje1]:[eje4]])</f>
-        <v>8.25</v>
+        <v>9.5</v>
       </c>
       <c r="N15" s="3">
         <f>IF(entregados[[#This Row],[calificación ]]&lt;10,IF((entregados[[#This Row],[calificación ]] + AVERAGE(entregados[[#This Row],[bienvenida]:[hipotesis]])/20)&gt;10,10, entregados[[#This Row],[calificación ]] + AVERAGE(entregados[[#This Row],[bienvenida]:[hipotesis]])/20), 10)</f>
-        <v>8.6387053571428574</v>
+        <v>9.8887053571428574</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>39</v>

</xml_diff>